<commit_message>
feat: styling of AI RMF
</commit_message>
<xml_diff>
--- a/src/assets/Muad-dib-ai.xlsx
+++ b/src/assets/Muad-dib-ai.xlsx
@@ -14,7 +14,7 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="75" uniqueCount="68">
   <si>
-    <t>##Govern-1: Policies, processes, procedures and practices across the organization related to the mapping, measuring and managing of AI risks are in place, transparent, and implemented effectively</t>
+    <t>Govern-1: Policies, processes, procedures and practices across the organization related to the mapping, measuring and managing of AI risks are in place, transparent, and implemented effectively</t>
   </si>
   <si>
     <t>Governance and Oversight</t>
@@ -36,12 +36,14 @@
 * Maintain policies for training (and re-training) organizational staff about necessary legal or regulatory considerations that may impact AI-related design, development and deployment activities.</t>
   </si>
   <si>
-    <t>### Organizations can document the following
+    <t>Organizations can document the following
+------------------------------
 - To what extent has the entity defined and documented the regulatory environmentâ€”including minimum requirements in laws and regulations?
 - Has the system been reviewed for its compliance to applicable laws, regulations, standards, and guidance? 
 - To what extent has the entity defined and documented the regulatory environmentâ€”including applicable requirements in laws and regulations? 
 - Has the system been reviewed for its compliance to relevant applicable laws, regulations, standards, and guidance? 
-### AI Transparency Resources
+AI Transparency Resources
+-------------------------------------------
 GAO-21-519SP: AI Accountability Framework for Federal Agencies &amp; Other Entities. [URL](https://www.gao.gov/products/gao-21-519sp)</t>
   </si>
   <si>

</xml_diff>